<commit_message>
Add complete clean dataset
</commit_message>
<xml_diff>
--- a/Data/Resources/Miscellaneous/COVID19 Data Dictionaries/Descriptores_071020.xlsx
+++ b/Data/Resources/Miscellaneous/COVID19 Data Dictionaries/Descriptores_071020.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ulise\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://purdue0-my.sharepoint.com/personal/jocegued_purdue_edu/Documents/Data Analytics Boot Camp/Projects/Project 2/covid-19-mexico-challenge/Data/Resources/Miscellaneous/COVID19 Data Dictionaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F2D96F-E63A-4FA0-A195-8D0A28DF91CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -765,20 +774,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B33" zoomScale="145" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="145" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="6"/>
+    <col min="1" max="1" width="9.1640625" style="6"/>
     <col min="2" max="2" width="26" style="7" customWidth="1"/>
-    <col min="3" max="3" width="47.109375" style="8" customWidth="1"/>
-    <col min="4" max="4" width="41.88671875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="47.1640625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="41.83203125" style="7" customWidth="1"/>
     <col min="5" max="5" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="29.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -792,7 +801,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -806,7 +815,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -820,7 +829,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="100.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -834,7 +843,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -848,7 +857,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -862,7 +871,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -876,7 +885,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -890,7 +899,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -904,7 +913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -918,7 +927,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -932,7 +941,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -946,7 +955,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -960,7 +969,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -974,7 +983,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -988,7 +997,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1002,7 +1011,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1016,7 +1025,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1030,7 +1039,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1044,7 +1053,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1058,7 +1067,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9">
         <v>20</v>
       </c>
@@ -1072,7 +1081,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1086,7 +1095,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1100,7 +1109,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1114,7 +1123,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1128,7 +1137,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1142,7 +1151,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1156,7 +1165,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1170,7 +1179,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1184,7 +1193,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1198,7 +1207,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1212,7 +1221,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1226,7 +1235,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9">
         <v>32</v>
       </c>
@@ -1240,7 +1249,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="9">
         <v>33</v>
       </c>
@@ -1254,7 +1263,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9">
         <v>34</v>
       </c>
@@ -1268,7 +1277,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1282,7 +1291,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="72.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -1296,7 +1305,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -1310,7 +1319,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1324,25 +1333,25 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
       <c r="B40" s="8"/>
       <c r="C40" s="7"/>
       <c r="D40"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="7"/>
       <c r="B41" s="8"/>
       <c r="C41" s="7"/>
       <c r="D41"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="7"/>
       <c r="B42" s="8"/>
       <c r="C42" s="7"/>
       <c r="D42"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="7"/>
       <c r="B43" s="8"/>
       <c r="C43" s="7"/>

</xml_diff>